<commit_message>
updated for 1 aug to 30 sep 2024
</commit_message>
<xml_diff>
--- a/01Aug2024 to 30Sep2024/AccountStatement1728988698744.xlsx
+++ b/01Aug2024 to 30Sep2024/AccountStatement1728988698744.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Statement Aug to Sep 2024" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Cheque Register" sheetId="2" r:id="rId3"/>
+    <sheet name="Cheque Register" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$D$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$B$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Statement Aug to Sep 2024'!$A$1:$D$86</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Txn Date</t>
   </si>
@@ -44,12 +44,6 @@
   <si>
     <t>y</t>
   </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
 </sst>
 </file>
 
@@ -59,7 +53,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="###0.00;###0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -78,14 +72,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +83,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -140,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -165,7 +159,19 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -474,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -609,7 +615,7 @@
       <c r="A11" s="2">
         <v>45507</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="8">
         <v>11.8</v>
       </c>
       <c r="C11" s="3"/>
@@ -669,7 +675,7 @@
       <c r="A16" s="2">
         <v>45510</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="8">
         <v>5002.3599999999997</v>
       </c>
       <c r="C16" s="3"/>
@@ -789,7 +795,7 @@
       <c r="A26" s="2">
         <v>45521</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="8">
         <v>151.04</v>
       </c>
       <c r="C26" s="3"/>
@@ -873,7 +879,7 @@
       <c r="A33" s="2">
         <v>45523</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="8">
         <v>80.239999999999995</v>
       </c>
       <c r="C33" s="3"/>
@@ -1185,7 +1191,7 @@
       <c r="A59" s="2">
         <v>45541</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B59" s="8">
         <v>136.88</v>
       </c>
       <c r="C59" s="3"/>
@@ -1305,7 +1311,7 @@
       <c r="A69" s="2">
         <v>45545</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B69" s="8">
         <v>87.32</v>
       </c>
       <c r="C69" s="3"/>
@@ -1525,561 +1531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2">
-        <v>45505</v>
-      </c>
-      <c r="C2">
-        <v>42500</v>
-      </c>
-      <c r="D2">
-        <v>45505</v>
-      </c>
-      <c r="E2">
-        <v>255000</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3">
-        <v>45505</v>
-      </c>
-      <c r="C3">
-        <v>255000</v>
-      </c>
-      <c r="D3">
-        <v>45505</v>
-      </c>
-      <c r="E3">
-        <v>42500</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4">
-        <v>45506</v>
-      </c>
-      <c r="C4">
-        <v>5000</v>
-      </c>
-      <c r="D4">
-        <v>45506</v>
-      </c>
-      <c r="E4">
-        <v>25500</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>45506</v>
-      </c>
-      <c r="C5">
-        <v>25500</v>
-      </c>
-      <c r="D5">
-        <v>45506</v>
-      </c>
-      <c r="E5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>45506</v>
-      </c>
-      <c r="C6">
-        <v>122294</v>
-      </c>
-      <c r="D6">
-        <v>45506</v>
-      </c>
-      <c r="E6">
-        <v>19500</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7">
-        <v>45507</v>
-      </c>
-      <c r="C7">
-        <v>64500</v>
-      </c>
-      <c r="D7">
-        <v>45506</v>
-      </c>
-      <c r="E7">
-        <v>64500</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8">
-        <v>45507</v>
-      </c>
-      <c r="C8">
-        <v>19500</v>
-      </c>
-      <c r="D8">
-        <v>45506</v>
-      </c>
-      <c r="E8">
-        <v>122294</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9">
-        <v>45507</v>
-      </c>
-      <c r="C9">
-        <v>11.8</v>
-      </c>
-      <c r="D9">
-        <v>45510</v>
-      </c>
-      <c r="E9">
-        <v>5002.3599999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10">
-        <v>45510</v>
-      </c>
-      <c r="C10">
-        <v>33815</v>
-      </c>
-      <c r="D10">
-        <v>45510</v>
-      </c>
-      <c r="E10">
-        <v>33815</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11">
-        <v>45510</v>
-      </c>
-      <c r="C11">
-        <v>49747</v>
-      </c>
-      <c r="D11">
-        <v>45510</v>
-      </c>
-      <c r="E11">
-        <v>49747</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12">
-        <v>45510</v>
-      </c>
-      <c r="C12">
-        <v>172362</v>
-      </c>
-      <c r="D12">
-        <v>45510</v>
-      </c>
-      <c r="E12">
-        <v>172362</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13">
-        <v>45510</v>
-      </c>
-      <c r="C13">
-        <v>5002.3599999999997</v>
-      </c>
-      <c r="D13">
-        <v>45516</v>
-      </c>
-      <c r="E13">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14">
-        <v>45518</v>
-      </c>
-      <c r="C14">
-        <v>1000000</v>
-      </c>
-      <c r="D14">
-        <v>45520</v>
-      </c>
-      <c r="E14">
-        <v>62315</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>45521</v>
-      </c>
-      <c r="C15">
-        <v>57170</v>
-      </c>
-      <c r="D15">
-        <v>45520</v>
-      </c>
-      <c r="E15">
-        <v>57170</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>45521</v>
-      </c>
-      <c r="C16">
-        <v>62315</v>
-      </c>
-      <c r="D16">
-        <v>45521</v>
-      </c>
-      <c r="E16">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>45521</v>
-      </c>
-      <c r="C17">
-        <v>151.04</v>
-      </c>
-      <c r="D17">
-        <v>45523</v>
-      </c>
-      <c r="E17">
-        <v>20310</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>45521</v>
-      </c>
-      <c r="C18">
-        <v>5002.3599999999997</v>
-      </c>
-      <c r="D18">
-        <v>45523</v>
-      </c>
-      <c r="E18">
-        <v>21225</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>45523</v>
-      </c>
-      <c r="C19">
-        <v>21225</v>
-      </c>
-      <c r="D19">
-        <v>45525</v>
-      </c>
-      <c r="E19">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>45523</v>
-      </c>
-      <c r="C20">
-        <v>20310</v>
-      </c>
-      <c r="D20">
-        <v>45525</v>
-      </c>
-      <c r="E20">
-        <v>14280</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>45523</v>
-      </c>
-      <c r="C21">
-        <v>80.239999999999995</v>
-      </c>
-      <c r="D21">
-        <v>45532</v>
-      </c>
-      <c r="E21">
-        <v>172362</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>45525</v>
-      </c>
-      <c r="C22">
-        <v>14280</v>
-      </c>
-      <c r="D22">
-        <v>45533</v>
-      </c>
-      <c r="E22">
-        <v>73700</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>45525</v>
-      </c>
-      <c r="C23">
-        <v>2500</v>
-      </c>
-      <c r="D23">
-        <v>45535</v>
-      </c>
-      <c r="E23">
-        <v>137250</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>45532</v>
-      </c>
-      <c r="C24">
-        <v>172362</v>
-      </c>
-      <c r="D24">
-        <v>45535</v>
-      </c>
-      <c r="E24">
-        <v>31046</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25">
-        <v>45535</v>
-      </c>
-      <c r="C25">
-        <v>137250</v>
-      </c>
-      <c r="D25">
-        <v>45538</v>
-      </c>
-      <c r="E25">
-        <v>29875</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26">
-        <v>45535</v>
-      </c>
-      <c r="C26">
-        <v>31046</v>
-      </c>
-      <c r="D26">
-        <v>45540</v>
-      </c>
-      <c r="E26">
-        <v>114908</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27">
-        <v>45537</v>
-      </c>
-      <c r="C27">
-        <v>73700</v>
-      </c>
-      <c r="D27">
-        <v>45540</v>
-      </c>
-      <c r="E27">
-        <v>35510</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28">
-        <v>45540</v>
-      </c>
-      <c r="C28">
-        <v>29875</v>
-      </c>
-      <c r="D28">
-        <v>45544</v>
-      </c>
-      <c r="E28">
-        <v>36285</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29">
-        <v>45540</v>
-      </c>
-      <c r="C29">
-        <v>114908</v>
-      </c>
-      <c r="D29">
-        <v>45544</v>
-      </c>
-      <c r="E29">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30">
-        <v>45541</v>
-      </c>
-      <c r="C30">
-        <v>35510</v>
-      </c>
-      <c r="D30">
-        <v>45546</v>
-      </c>
-      <c r="E30">
-        <v>13415</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31">
-        <v>45541</v>
-      </c>
-      <c r="C31">
-        <v>136.88</v>
-      </c>
-      <c r="D31">
-        <v>45551</v>
-      </c>
-      <c r="E31">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32">
-        <v>45544</v>
-      </c>
-      <c r="C32">
-        <v>1115</v>
-      </c>
-      <c r="D32">
-        <v>45555</v>
-      </c>
-      <c r="E32">
-        <v>10300</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33">
-        <v>45545</v>
-      </c>
-      <c r="C33">
-        <v>36285</v>
-      </c>
-      <c r="D33">
-        <v>45562</v>
-      </c>
-      <c r="E33">
-        <v>14550</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34">
-        <v>45545</v>
-      </c>
-      <c r="C34">
-        <v>87.32</v>
-      </c>
-      <c r="D34">
-        <v>45565</v>
-      </c>
-      <c r="E34">
-        <v>31046</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35">
-        <v>45546</v>
-      </c>
-      <c r="C35">
-        <v>13415</v>
-      </c>
-      <c r="D35">
-        <v>45565</v>
-      </c>
-      <c r="E35">
-        <v>28228</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36">
-        <v>45551</v>
-      </c>
-      <c r="C36">
-        <v>75000</v>
-      </c>
-      <c r="D36">
-        <v>45565</v>
-      </c>
-      <c r="E36">
-        <v>105750</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37">
-        <v>45556</v>
-      </c>
-      <c r="C37">
-        <v>10300</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38">
-        <v>45562</v>
-      </c>
-      <c r="C38">
-        <v>14550</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39">
-        <v>45565</v>
-      </c>
-      <c r="C39">
-        <v>105750</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40">
-        <v>45565</v>
-      </c>
-      <c r="C40">
-        <v>31046</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B36"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
@@ -2153,11 +1608,11 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>45510</v>
-      </c>
-      <c r="B9" s="6">
-        <v>5002.3599999999997</v>
+      <c r="A9" s="9">
+        <v>45507</v>
+      </c>
+      <c r="B9" s="11">
+        <v>11.8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2165,7 +1620,7 @@
         <v>45510</v>
       </c>
       <c r="B10" s="6">
-        <v>33815</v>
+        <v>5002.3599999999997</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2173,7 +1628,7 @@
         <v>45510</v>
       </c>
       <c r="B11" s="6">
-        <v>49747</v>
+        <v>33815</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2181,202 +1636,1327 @@
         <v>45510</v>
       </c>
       <c r="B12" s="6">
-        <v>172362</v>
+        <v>49747</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
-        <v>45516</v>
+        <v>45510</v>
       </c>
       <c r="B13" s="6">
-        <v>1000000</v>
+        <v>172362</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>45520</v>
-      </c>
-      <c r="B14" s="6">
-        <v>62315</v>
+      <c r="A14" s="9">
+        <v>45510</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2.36</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
-        <v>45520</v>
+        <v>45516</v>
       </c>
       <c r="B15" s="6">
-        <v>57170</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
-        <v>45521</v>
+        <v>45520</v>
       </c>
       <c r="B16" s="6">
-        <v>5000</v>
+        <v>62315</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
-        <v>45523</v>
+        <v>45520</v>
       </c>
       <c r="B17" s="6">
-        <v>20310</v>
+        <v>57170</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
-        <v>45523</v>
+        <v>45521</v>
       </c>
       <c r="B18" s="6">
-        <v>21225</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>45525</v>
-      </c>
-      <c r="B19" s="6">
-        <v>2500</v>
+      <c r="A19" s="9">
+        <v>45521</v>
+      </c>
+      <c r="B19" s="11">
+        <v>151.04</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
-        <v>45525</v>
+        <v>45523</v>
       </c>
       <c r="B20" s="6">
-        <v>14280</v>
+        <v>20310</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
-        <v>45532</v>
+        <v>45523</v>
       </c>
       <c r="B21" s="6">
-        <v>172362</v>
+        <v>21225</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>45533</v>
-      </c>
-      <c r="B22" s="6">
-        <v>73700</v>
+      <c r="A22" s="9">
+        <v>45523</v>
+      </c>
+      <c r="B22" s="11">
+        <v>80.239999999999995</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
-        <v>45535</v>
+        <v>45525</v>
       </c>
       <c r="B23" s="6">
-        <v>137250</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
-        <v>45535</v>
+        <v>45525</v>
       </c>
       <c r="B24" s="6">
-        <v>31046</v>
+        <v>14280</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
-        <v>45538</v>
+        <v>45532</v>
       </c>
       <c r="B25" s="6">
-        <v>29875</v>
+        <v>172362</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
-        <v>45540</v>
+        <v>45533</v>
       </c>
       <c r="B26" s="6">
-        <v>114908</v>
+        <v>73700</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
-        <v>45540</v>
+        <v>45535</v>
       </c>
       <c r="B27" s="6">
-        <v>35510</v>
+        <v>137250</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
-        <v>45544</v>
+        <v>45535</v>
       </c>
       <c r="B28" s="6">
-        <v>36285</v>
+        <v>31046</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
-        <v>45544</v>
+        <v>45538</v>
       </c>
       <c r="B29" s="6">
-        <v>1115</v>
+        <v>29875</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
-        <v>45546</v>
+        <v>45540</v>
       </c>
       <c r="B30" s="6">
-        <v>13415</v>
+        <v>114908</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
-        <v>45551</v>
+        <v>45540</v>
       </c>
       <c r="B31" s="6">
-        <v>75000</v>
+        <v>35510</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>45555</v>
-      </c>
-      <c r="B32" s="6">
-        <v>10300</v>
+      <c r="A32" s="9">
+        <v>45541</v>
+      </c>
+      <c r="B32" s="11">
+        <v>136.88</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
-        <v>45562</v>
+        <v>45544</v>
       </c>
       <c r="B33" s="6">
-        <v>14550</v>
+        <v>36285</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
-        <v>45565</v>
+        <v>45544</v>
       </c>
       <c r="B34" s="6">
-        <v>31046</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>45565</v>
-      </c>
-      <c r="B35" s="6">
-        <v>28228</v>
+      <c r="A35" s="9">
+        <v>45545</v>
+      </c>
+      <c r="B35" s="11">
+        <v>87.32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
+        <v>45546</v>
+      </c>
+      <c r="B36" s="6">
+        <v>13415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
+        <v>45551</v>
+      </c>
+      <c r="B37" s="12">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10">
+        <v>45555</v>
+      </c>
+      <c r="B38" s="12">
+        <v>10300</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10">
+        <v>45562</v>
+      </c>
+      <c r="B39" s="12">
+        <v>14550</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10">
         <v>45565</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B40" s="12">
+        <v>31046</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10">
+        <v>45565</v>
+      </c>
+      <c r="B41" s="12">
+        <v>28228</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10">
+        <v>45565</v>
+      </c>
+      <c r="B42" s="12">
         <v>105750</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>45505</v>
+      </c>
+      <c r="B2">
+        <v>-255000</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"["&amp;A2&amp;","&amp;B2&amp;"],"</f>
+        <v>[45505,-255000],</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>45505</v>
+      </c>
+      <c r="B3">
+        <v>-42500</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="0">"["&amp;A3&amp;","&amp;B3&amp;"],"</f>
+        <v>[45505,-42500],</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>45505</v>
+      </c>
+      <c r="B4">
+        <v>230</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>[45505,230],</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>45506</v>
+      </c>
+      <c r="B5">
+        <v>-25500</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>[45506,-25500],</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>45506</v>
+      </c>
+      <c r="B6">
+        <v>-5000</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>[45506,-5000],</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>45506</v>
+      </c>
+      <c r="B7">
+        <v>-19500</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>[45506,-19500],</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>45506</v>
+      </c>
+      <c r="B8">
+        <v>-64500</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>[45506,-64500],</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>45506</v>
+      </c>
+      <c r="B9">
+        <v>-122294</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>[45506,-122294],</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>45507</v>
+      </c>
+      <c r="B10">
+        <v>-11.8</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>[45507,-11.8],</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>45507</v>
+      </c>
+      <c r="B11">
+        <v>1480</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>[45507,1480],</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45510</v>
+      </c>
+      <c r="B12">
+        <v>-5002.3599999999997</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,-5002.36],</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>45510</v>
+      </c>
+      <c r="B13">
+        <v>-33815</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,-33815],</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>45510</v>
+      </c>
+      <c r="B14">
+        <v>-49747</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,-49747],</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>45510</v>
+      </c>
+      <c r="B15">
+        <v>-172362</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,-172362],</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>45510</v>
+      </c>
+      <c r="B16">
+        <v>-2.36</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,-2.36],</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>45510</v>
+      </c>
+      <c r="B17">
+        <v>3200</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>[45510,3200],</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>45511</v>
+      </c>
+      <c r="B18">
+        <v>460</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>[45511,460],</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>45513</v>
+      </c>
+      <c r="B19">
+        <v>1360</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>[45513,1360],</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>45514</v>
+      </c>
+      <c r="B20">
+        <v>630</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>[45514,630],</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>45516</v>
+      </c>
+      <c r="B21">
+        <v>-1000000</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>[45516,-1000000],</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>45517</v>
+      </c>
+      <c r="B22">
+        <v>660</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>[45517,660],</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>45518</v>
+      </c>
+      <c r="B23">
+        <v>800</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>[45518,800],</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>45519</v>
+      </c>
+      <c r="B24">
+        <v>1800</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>[45519,1800],</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>45520</v>
+      </c>
+      <c r="B25">
+        <v>-62315</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>[45520,-62315],</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>45520</v>
+      </c>
+      <c r="B26">
+        <v>-57170</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>[45520,-57170],</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>45521</v>
+      </c>
+      <c r="B27">
+        <v>-5000</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>[45521,-5000],</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>45521</v>
+      </c>
+      <c r="B28">
+        <v>-151.04</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>[45521,-151.04],</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>45523</v>
+      </c>
+      <c r="B29">
+        <v>-20310</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,-20310],</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>45523</v>
+      </c>
+      <c r="B30">
+        <v>-21225</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,-21225],</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>45523</v>
+      </c>
+      <c r="B31">
+        <v>-80.239999999999995</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,-80.24],</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>45523</v>
+      </c>
+      <c r="B32">
+        <v>1800</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,1800],</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>45523</v>
+      </c>
+      <c r="B33">
+        <v>335</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,335],</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>45523</v>
+      </c>
+      <c r="B34">
+        <v>2335</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,2335],</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>45523</v>
+      </c>
+      <c r="B35">
+        <v>8255</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>[45523,8255],</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>45524</v>
+      </c>
+      <c r="B36">
+        <v>230</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>[45524,230],</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>45524</v>
+      </c>
+      <c r="B37">
+        <v>4080</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>[45524,4080],</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>45525</v>
+      </c>
+      <c r="B38">
+        <v>-2500</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>[45525,-2500],</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>45525</v>
+      </c>
+      <c r="B39">
+        <v>-14280</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>[45525,-14280],</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>45525</v>
+      </c>
+      <c r="B40">
+        <v>230</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>[45525,230],</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>45526</v>
+      </c>
+      <c r="B41">
+        <v>460</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>[45526,460],</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>45527</v>
+      </c>
+      <c r="B42">
+        <v>2800</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>[45527,2800],</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>45527</v>
+      </c>
+      <c r="B43">
+        <v>7740</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>[45527,7740],</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>45528</v>
+      </c>
+      <c r="B44">
+        <v>2000</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>[45528,2000],</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45532</v>
+      </c>
+      <c r="B45">
+        <v>-172362</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>[45532,-172362],</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45533</v>
+      </c>
+      <c r="B46">
+        <v>-73700</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>[45533,-73700],</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>45533</v>
+      </c>
+      <c r="B47">
+        <v>600</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>[45533,600],</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>45535</v>
+      </c>
+      <c r="B48">
+        <v>-137250</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>[45535,-137250],</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>45535</v>
+      </c>
+      <c r="B49">
+        <v>-31046</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>[45535,-31046],</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>45535</v>
+      </c>
+      <c r="B50">
+        <v>560</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>[45535,560],</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>45536</v>
+      </c>
+      <c r="B51">
+        <v>800</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>[45536,800],</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>45538</v>
+      </c>
+      <c r="B52">
+        <v>-29875</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>[45538,-29875],</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>45539</v>
+      </c>
+      <c r="B53">
+        <v>230</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>[45539,230],</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>45540</v>
+      </c>
+      <c r="B54">
+        <v>-114908</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>[45540,-114908],</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>45540</v>
+      </c>
+      <c r="B55">
+        <v>-35510</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>[45540,-35510],</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>45540</v>
+      </c>
+      <c r="B56">
+        <v>270</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>[45540,270],</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>45540</v>
+      </c>
+      <c r="B57">
+        <v>180</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>[45540,180],</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>45540</v>
+      </c>
+      <c r="B58">
+        <v>80</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>[45540,80],</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>45541</v>
+      </c>
+      <c r="B59">
+        <v>-136.88</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>[45541,-136.88],</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>45541</v>
+      </c>
+      <c r="B60">
+        <v>690</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>[45541,690],</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>45542</v>
+      </c>
+      <c r="B61">
+        <v>2230</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>[45542,2230],</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>45542</v>
+      </c>
+      <c r="B62">
+        <v>7900</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>[45542,7900],</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>45544</v>
+      </c>
+      <c r="B63">
+        <v>-36285</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>[45544,-36285],</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>45544</v>
+      </c>
+      <c r="B64">
+        <v>-1115</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>[45544,-1115],</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>45544</v>
+      </c>
+      <c r="B65">
+        <v>1600</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>[45544,1600],</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>45544</v>
+      </c>
+      <c r="B66">
+        <v>110</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>[45544,110],</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>45544</v>
+      </c>
+      <c r="B67">
+        <v>9200</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67:D88" si="1">"["&amp;A67&amp;","&amp;B67&amp;"],"</f>
+        <v>[45544,9200],</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>45545</v>
+      </c>
+      <c r="B68">
+        <v>-87.32</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>[45545,-87.32],</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>45545</v>
+      </c>
+      <c r="B69">
+        <v>55</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>[45545,55],</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>45545</v>
+      </c>
+      <c r="B70">
+        <v>1030</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>[45545,1030],</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>45546</v>
+      </c>
+      <c r="B71">
+        <v>-13415</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>[45546,-13415],</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>45546</v>
+      </c>
+      <c r="B72">
+        <v>1950</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>[45546,1950],</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>45546</v>
+      </c>
+      <c r="B73">
+        <v>375</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>[45546,375],</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>45547</v>
+      </c>
+      <c r="B74">
+        <v>230</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>[45547,230],</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>45551</v>
+      </c>
+      <c r="B75">
+        <v>-75000</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>[45551,-75000],</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>45552</v>
+      </c>
+      <c r="B76">
+        <v>460</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>[45552,460],</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>45555</v>
+      </c>
+      <c r="B77">
+        <v>-10300</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>[45555,-10300],</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>45556</v>
+      </c>
+      <c r="B78">
+        <v>400</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>[45556,400],</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>45557</v>
+      </c>
+      <c r="B79">
+        <v>230</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>[45557,230],</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>45559</v>
+      </c>
+      <c r="B80">
+        <v>800</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>[45559,800],</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>45560</v>
+      </c>
+      <c r="B81">
+        <v>1360</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>[45560,1360],</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>45560</v>
+      </c>
+      <c r="B82">
+        <v>48060</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>[45560,48060],</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>45561</v>
+      </c>
+      <c r="B83">
+        <v>2230</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>[45561,2230],</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>45562</v>
+      </c>
+      <c r="B84">
+        <v>-14550</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>[45562,-14550],</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>45563</v>
+      </c>
+      <c r="B85">
+        <v>630</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>[45563,630],</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>45565</v>
+      </c>
+      <c r="B86">
+        <v>-31046</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>[45565,-31046],</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>45565</v>
+      </c>
+      <c r="B87">
+        <v>-28228</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>[45565,-28228],</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>45565</v>
+      </c>
+      <c r="B88">
+        <v>-105750</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>[45565,-105750],</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B88">
+    <sortCondition ref="A2:A88"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>